<commit_message>
Save changes before implementing dynamic form customization
</commit_message>
<xml_diff>
--- a/media/sample_asset_upload.xlsx
+++ b/media/sample_asset_upload.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://oilindia-my.sharepoint.com/personal/tituraj_doley_oilindia_in/Documents/Desktop/IT Portal/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://oilindia-my.sharepoint.com/personal/tituraj_doley_oilindia_in/Documents/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="9" documentId="11_D7521ECD97D9AE2F0A565F38972F4FD961B4FCA0" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{92A1ECBA-AD28-434E-9967-47489CCE5412}"/>
+  <xr:revisionPtr revIDLastSave="6" documentId="11_95A7818FF9F66F0C0E993433E81AC271C82C8C1E" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{85E7C2B1-09AB-491C-BACF-712EB109DA53}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>serial_number</t>
   </si>
@@ -37,76 +37,16 @@
     <t>installation_date</t>
   </si>
   <si>
-    <t>warranty_start_date</t>
-  </si>
-  <si>
-    <t>warranty_end_date</t>
-  </si>
-  <si>
-    <t>warranty_provider</t>
-  </si>
-  <si>
-    <t>amc_start_date</t>
-  </si>
-  <si>
-    <t>amc_end_date</t>
-  </si>
-  <si>
-    <t>amc_provider</t>
-  </si>
-  <si>
-    <t>12345</t>
-  </si>
-  <si>
-    <t>67890</t>
-  </si>
-  <si>
-    <t>Computer</t>
-  </si>
-  <si>
-    <t>Laptop</t>
-  </si>
-  <si>
-    <t>PO001</t>
-  </si>
-  <si>
-    <t>PO002</t>
-  </si>
-  <si>
-    <t>SAP1234</t>
-  </si>
-  <si>
-    <t>SAP5678</t>
-  </si>
-  <si>
-    <t>2025-01-01</t>
-  </si>
-  <si>
-    <t>2025-02-01</t>
-  </si>
-  <si>
-    <t>2026-01-01</t>
-  </si>
-  <si>
-    <t>2026-02-01</t>
-  </si>
-  <si>
-    <t>Dell</t>
-  </si>
-  <si>
-    <t>HP</t>
-  </si>
-  <si>
-    <t>2025-03-01</t>
-  </si>
-  <si>
-    <t>2025-12-31</t>
-  </si>
-  <si>
-    <t>2026-12-31</t>
-  </si>
-  <si>
-    <t>Lenovo</t>
+    <t>amc_contract</t>
+  </si>
+  <si>
+    <t>end_user</t>
+  </si>
+  <si>
+    <t>laptop</t>
+  </si>
+  <si>
+    <t>Tituraj</t>
   </si>
 </sst>
 </file>
@@ -185,6 +125,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -474,26 +418,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K3"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:F1048576"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
+    <col min="1" max="1" width="13" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.90625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.6328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.6328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.08984375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.453125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.6328125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.1796875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.36328125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -515,87 +452,19 @@
       <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>12345</v>
+      </c>
+      <c r="B2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="F2">
+        <v>611888</v>
+      </c>
+      <c r="G2" t="s">
         <v>8</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G2" t="s">
-        <v>21</v>
-      </c>
-      <c r="H2" t="s">
-        <v>23</v>
-      </c>
-      <c r="I2" t="s">
-        <v>20</v>
-      </c>
-      <c r="J2" t="s">
-        <v>26</v>
-      </c>
-      <c r="K2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E3" t="s">
-        <v>20</v>
-      </c>
-      <c r="F3" t="s">
-        <v>20</v>
-      </c>
-      <c r="G3" t="s">
-        <v>22</v>
-      </c>
-      <c r="H3" t="s">
-        <v>24</v>
-      </c>
-      <c r="I3" t="s">
-        <v>25</v>
-      </c>
-      <c r="J3" t="s">
-        <v>27</v>
-      </c>
-      <c r="K3" t="s">
-        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>